<commit_message>
Added code to initialize an order for each trade. trade constructor calls order.setMainOrderFields. Still need to handle the messages in response to order placement (orderStatus, execDetails.. something like that)
changed watchlist.txt to watchlist.csv. Much easier to parse out now.
</commit_message>
<xml_diff>
--- a/watchList.xlsx
+++ b/watchList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>OPT</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>FB</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -418,15 +421,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -440,28 +446,32 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -475,33 +485,36 @@
         <v>95</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>20160624</v>
+      <c r="H2" t="s">
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>94</v>
-      </c>
-      <c r="J2" t="s">
+        <v>20161021</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2">
-        <v>232384443</v>
+      <c r="L2">
+        <v>215606586</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C3">
         <v>115</v>
@@ -510,12 +523,15 @@
         <v>103</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
found bug in trade.initOrder
</commit_message>
<xml_diff>
--- a/watchList.xlsx
+++ b/watchList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="1440" windowWidth="19320" windowHeight="10000" tabRatio="500"/>
+    <workbookView xWindow="6140" yWindow="460" windowWidth="22660" windowHeight="10000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="watchList.txt" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>OPT</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -421,18 +424,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -455,23 +458,26 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -493,23 +499,26 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>20161021</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>100</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>215606586</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -531,7 +540,10 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>